<commit_message>
Adding Quotation POM and TSs
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/quotations.xlsx
+++ b/src/main/resources/excel/quotations.xlsx
@@ -1,32 +1,119 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="14835" windowHeight="6420"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+  <si>
+    <t>TestCaseID</t>
+  </si>
+  <si>
+    <t>TestData1</t>
+  </si>
+  <si>
+    <t>TestData2</t>
+  </si>
+  <si>
+    <t>TestData3</t>
+  </si>
+  <si>
+    <t>TestData4</t>
+  </si>
+  <si>
+    <t>TestData5</t>
+  </si>
+  <si>
+    <t>CreateQuoteWithStageAccepted</t>
+  </si>
+  <si>
+    <t>quote14</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>CreateQuoteWithStagerejected</t>
+  </si>
+  <si>
+    <t>quote15</t>
+  </si>
+  <si>
+    <t>Rejected</t>
+  </si>
+  <si>
+    <t>CreateQuoteWithContact</t>
+  </si>
+  <si>
+    <t>quote16</t>
+  </si>
+  <si>
+    <t>pradeep sharma</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>CreateQuoteWithOrganisation</t>
+  </si>
+  <si>
+    <t>quote17</t>
+  </si>
+  <si>
+    <t>ValidateQuoteNo</t>
+  </si>
+  <si>
+    <t>Quote No</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>QUO20</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -49,8 +136,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -111,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -146,7 +236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -323,20 +413,139 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75">
+      <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>